<commit_message>
Updated excel with coresponding tests and colorcodes.
</commit_message>
<xml_diff>
--- a/CSCI306_MAP.xlsx
+++ b/CSCI306_MAP.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\CSCI306\ClueGameJLRG\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,127 +24,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="37">
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAIN DECK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEDICAL BAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREW QUARTERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGINE ROOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHUTTLE BAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSPORTER ROOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GREENHOUSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIRK'S OFFICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OFFICER'S QUARTERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WALKWAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOORWAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ER</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="42">
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>KL</t>
+  </si>
+  <si>
+    <t>MAIN DECK</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>MEDICAL BAY</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CREW QUARTERS</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>ENGINE ROOM</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SHUTTLE BAY</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>TRANSPORTER ROOM</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GREENHOUSE</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>KIRK'S OFFICE</t>
+  </si>
+  <si>
+    <t>OFFICER'S QUARTERS</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>WALKWAY</t>
+  </si>
+  <si>
+    <t>DOORWAY</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>ROOM</t>
+  </si>
+  <si>
+    <t>CLOSET</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list test, inside room</t>
+  </si>
+  <si>
+    <t>Purple: adjacency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Gold: walkway scenarios</t>
+  </si>
+  <si>
+    <t>Light green: test targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -148,23 +164,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,9 +196,45 @@
         <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -205,61 +242,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -318,49 +321,322 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AA25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U14" activeCellId="0" sqref="U14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.89068825910931"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.67611336032389"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="2.89068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.31983805668016"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.42914979757085"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="3.31983805668016"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="2.89068825910931"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="3.42914979757085"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="2.89068825910931"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="3.64372469635628"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="3.10526315789474"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="3.64372469635628"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="3.53441295546559"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="2.85546875"/>
+    <col min="2" max="3" width="3.140625"/>
+    <col min="4" max="4" width="3.5703125"/>
+    <col min="5" max="5" width="3.140625"/>
+    <col min="6" max="6" width="2.7109375"/>
+    <col min="7" max="9" width="2.85546875"/>
+    <col min="10" max="10" width="3.28515625"/>
+    <col min="11" max="11" width="3.42578125"/>
+    <col min="12" max="12" width="3.5703125"/>
+    <col min="13" max="13" width="3.140625"/>
+    <col min="14" max="15" width="3.28515625"/>
+    <col min="16" max="18" width="2.85546875"/>
+    <col min="19" max="19" width="3"/>
+    <col min="20" max="20" width="3.42578125"/>
+    <col min="21" max="21" width="2.85546875"/>
+    <col min="22" max="22" width="3.5703125"/>
+    <col min="23" max="23" width="3.140625"/>
+    <col min="24" max="25" width="3.5703125"/>
+    <col min="26" max="26" width="8.5703125"/>
+    <col min="27" max="27" width="22.28515625"/>
+    <col min="28" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +658,7 @@
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -430,14 +706,14 @@
       <c r="W1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="0" t="n">
+      <c r="Y1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +771,7 @@
       <c r="S2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="U2" s="1" t="s">
@@ -510,17 +786,17 @@
       <c r="X2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="0" t="s">
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +809,7 @@
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -593,17 +869,17 @@
       <c r="X3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="0" t="s">
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,7 +937,7 @@
       <c r="S4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="U4" s="2" t="s">
@@ -670,23 +946,23 @@
       <c r="V4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4">
         <v>3</v>
       </c>
-      <c r="Z4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA4" s="0" t="s">
+      <c r="Z4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +1017,7 @@
       <c r="R5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -759,24 +1035,24 @@
       <c r="X5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="Y5">
         <v>4</v>
       </c>
-      <c r="Z5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA5" s="0" t="s">
+      <c r="Z5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -842,17 +1118,17 @@
       <c r="X6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y6" s="0" t="n">
+      <c r="Y6">
         <v>5</v>
       </c>
-      <c r="Z6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA6" s="0" t="s">
+      <c r="Z6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -925,18 +1201,18 @@
       <c r="X7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y7" s="0" t="n">
+      <c r="Y7">
         <v>6</v>
       </c>
-      <c r="Z7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA7" s="0" t="s">
+      <c r="Z7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -945,7 +1221,7 @@
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1008,24 +1284,24 @@
       <c r="X8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="0" t="n">
+      <c r="Y8">
         <v>7</v>
       </c>
-      <c r="Z8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="0" t="s">
+      <c r="Z8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1067,7 +1343,7 @@
       <c r="P9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -1085,23 +1361,23 @@
       <c r="V9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="W9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z9" s="0" t="s">
+      <c r="Y9">
+        <v>8</v>
+      </c>
+      <c r="Z9" t="s">
         <v>3</v>
       </c>
-      <c r="AA9" s="0" t="s">
+      <c r="AA9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1171,20 +1447,20 @@
       <c r="W10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="0" t="n">
+      <c r="X10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10">
         <v>9</v>
       </c>
-      <c r="Z10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA10" s="0" t="s">
+      <c r="Z10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1257,11 +1533,11 @@
       <c r="X11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y11" s="0" t="n">
+      <c r="Y11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1334,14 +1610,14 @@
       <c r="X12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="0" t="n">
+      <c r="Y12">
         <v>11</v>
       </c>
       <c r="AA12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1414,14 +1690,14 @@
       <c r="X13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y13" s="0" t="n">
+      <c r="Y13">
         <v>12</v>
       </c>
       <c r="AA13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1431,7 +1707,7 @@
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1482,7 +1758,7 @@
       <c r="T14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="U14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="V14" s="1" t="s">
@@ -1494,15 +1770,15 @@
       <c r="X14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y14" s="0" t="n">
+      <c r="Y14">
         <v>13</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1574,14 +1850,14 @@
       <c r="X15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y15" s="0" t="n">
+      <c r="Y15">
         <v>14</v>
       </c>
       <c r="AA15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -1627,7 +1903,7 @@
       <c r="O16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P16" s="8" t="s">
         <v>1</v>
       </c>
       <c r="Q16" s="2" t="s">
@@ -1654,11 +1930,11 @@
       <c r="X16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y16" s="0" t="n">
+      <c r="Y16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1692,7 +1968,7 @@
       <c r="K17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="M17" s="1" t="s">
@@ -1731,11 +2007,11 @@
       <c r="X17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y17" s="0" t="n">
+      <c r="Y17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1778,7 +2054,7 @@
       <c r="N18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="P18" s="2" t="s">
@@ -1799,7 +2075,7 @@
       <c r="U18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="V18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="W18" s="1" t="s">
@@ -1808,11 +2084,11 @@
       <c r="X18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y18" s="0" t="n">
+      <c r="Y18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1861,7 +2137,7 @@
       <c r="P19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="Q19" s="9" t="s">
         <v>1</v>
       </c>
       <c r="R19" s="2" t="s">
@@ -1885,11 +2161,11 @@
       <c r="X19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y19" s="0" t="n">
+      <c r="Y19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1962,11 +2238,11 @@
       <c r="X20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y20" s="0" t="n">
+      <c r="Y20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1976,7 +2252,7 @@
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -2039,11 +2315,11 @@
       <c r="X21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y21" s="0" t="n">
+      <c r="Y21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2065,7 +2341,7 @@
       <c r="G22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2116,11 +2392,14 @@
       <c r="X22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y22" s="0" t="n">
+      <c r="Y22">
         <v>21</v>
       </c>
+      <c r="AA22" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -2193,11 +2472,14 @@
       <c r="X23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y23" s="0" t="n">
+      <c r="Y23">
         <v>22</v>
       </c>
+      <c r="AA23" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2243,10 +2525,10 @@
       <c r="O24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="2" t="s">
+      <c r="P24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -2270,91 +2552,97 @@
       <c r="X24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y24" s="0" t="n">
-        <v>23</v>
+      <c r="Y24">
+        <v>23</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" s="0" t="n">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
         <v>3</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25">
         <v>4</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>5</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25">
         <v>6</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25">
         <v>7</v>
       </c>
-      <c r="I25" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J25" s="0" t="n">
+      <c r="I25">
+        <v>8</v>
+      </c>
+      <c r="J25">
         <v>9</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25">
         <v>10</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25">
         <v>11</v>
       </c>
-      <c r="M25" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="O25" s="0" t="n">
+      <c r="M25">
+        <v>12</v>
+      </c>
+      <c r="N25">
+        <v>13</v>
+      </c>
+      <c r="O25">
         <v>14</v>
       </c>
-      <c r="P25" s="0" t="n">
+      <c r="P25">
         <v>15</v>
       </c>
-      <c r="Q25" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="R25" s="0" t="n">
+      <c r="Q25">
+        <v>16</v>
+      </c>
+      <c r="R25">
         <v>17</v>
       </c>
-      <c r="S25" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="T25" s="0" t="n">
+      <c r="S25">
+        <v>18</v>
+      </c>
+      <c r="T25">
         <v>19</v>
       </c>
-      <c r="U25" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="V25" s="0" t="n">
+      <c r="U25">
+        <v>20</v>
+      </c>
+      <c r="V25">
         <v>21</v>
       </c>
-      <c r="W25" s="0" t="n">
+      <c r="W25">
         <v>22</v>
       </c>
-      <c r="X25" s="0" t="n">
-        <v>23</v>
+      <c r="X25">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA26" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>